<commit_message>
add functional test case
</commit_message>
<xml_diff>
--- a/adhafera/test/function_test.xlsx
+++ b/adhafera/test/function_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -37,19 +37,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>テストモジュール</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テストケース</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>1.0.0</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>条件</t>
@@ -59,11 +47,392 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.0.0</t>
+    <t>操作</t>
+    <rPh sb="0" eb="2">
+      <t>ソウサ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリを起動</t>
+    <rPh sb="4" eb="6">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録ボタンを押下</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>状態</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていないこと
+・テーブルは'支出'が選択されていること</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>取消ボタンを押下</t>
+    <rPh sb="0" eb="2">
+      <t>トリケシ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: '2015-01-01'
+内容: 'テスト用データ'
+カテゴリ: 'テスト'
+金額: '100'
+ボタン: '収入'を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: '2015-01-01'
+内容: 'テスト用データ'
+ボタン: '収入'を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・入力欄には何も表示されていないこと
+・テーブルは'収入'が選択されていること</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・'家計簿が登録されました'と表示されていること
+・テーブルは'収入'が選択されていること</t>
+    <rPh sb="2" eb="5">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>シュウニュウ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: '2015-01-01'
+内容: 'テスト用データ'
+ボタン: '支出'を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・'カテゴリ, 金額を入力してください'と表示されていること
+・カテゴリの入力欄の横にマークが表示されていること
+・金額の入力欄の横にマークが表示されていること</t>
+    <rPh sb="8" eb="10">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="37" eb="40">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="61" eb="64">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・'日付が不正です'と表示されていること
+・日付の入力欄の横にマークが表示されていること</t>
+    <rPh sb="2" eb="4">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・'金額が不正です'と表示されていること
+・金額の入力欄の横にマークが表示されていること</t>
+    <rPh sb="2" eb="4">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: '不正な日付'
+内容: 'テスト用データ'
+カテゴリ: 'テスト'
+金額: '100'
+ボタン: '支出'を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: '2015-01-01'
+内容: 'テスト用データ'
+カテゴリ: 'テスト'
+金額: '不正な金額'
+ボタン: '支出'を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付: '01-01-2015'
+内容: 'テスト用データ'
+カテゴリ: 'テスト'
+金額: '-100'
+ボタン: '支出'を選択</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="60" eb="62">
+      <t>シシュツ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・'日付, 金額が不正です'と表示されていること
+・日付の入力欄の横にマークが表示されていること
+・金額の入力欄の横にマークが表示されていること</t>
+    <rPh sb="2" eb="4">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>フセイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="29" eb="32">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="53" eb="56">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>ヒョウジ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -120,7 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -245,43 +614,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -394,36 +726,16 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -607,20 +919,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -633,53 +951,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="189">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -771,6 +1068,9 @@
     <cellStyle name="ハイパーリンク" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -863,6 +1163,9 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1191,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G30"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1214,353 +1517,87 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" ht="31">
       <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
+      <c r="G3" s="15" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" ht="70">
       <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="15" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" ht="70">
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="15" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="8">
+    <row r="6" spans="2:7" ht="45" thickBot="1">
+      <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="8">
-        <v>8</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="8">
-        <v>9</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="8">
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="8">
-        <v>11</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="8">
+      <c r="E6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="8">
+      <c r="F6" s="18"/>
+      <c r="G6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="8">
-        <v>14</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="8">
-        <v>15</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="8">
-        <v>16</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="8">
-        <v>17</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="8">
-        <v>18</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="8">
-        <v>19</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="8">
-        <v>20</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="8">
-        <v>21</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="8">
-        <v>22</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="8">
-        <v>23</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="8">
-        <v>24</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="8">
-        <v>25</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="8">
-        <v>26</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="8">
-        <v>27</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="2:7" ht="19" thickBot="1">
-      <c r="B30" s="15">
-        <v>28</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1576,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G21"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1587,7 +1624,8 @@
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="4" max="4" width="47.1640625" customWidth="1"/>
     <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="7" width="47.1640625" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" customWidth="1"/>
+    <col min="7" max="7" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="19" thickBot="1"/>
@@ -1599,245 +1637,89 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="20">
+    <row r="3" spans="2:7" ht="44">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
+      <c r="G3" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="20">
+    <row r="4" spans="2:7" ht="70">
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="15" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="20">
+    <row r="5" spans="2:7" ht="70">
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="15" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="20">
+    <row r="6" spans="2:7" ht="71" thickBot="1">
+      <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="20">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="20">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="20">
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="20">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="20">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="20">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="20">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="20">
-        <v>12</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="20">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="20">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="20">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="20">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="20">
-        <v>17</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="20">
-        <v>18</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="2:7" ht="19" thickBot="1">
-      <c r="B21" s="15">
-        <v>19</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
+      <c r="E6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
create system test spec
</commit_message>
<xml_diff>
--- a/adhafera/test/function_test.xlsx
+++ b/adhafera/test/function_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -37,6 +37,14 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>テストモジュール</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テストケース</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>1.0.0</t>
   </si>
   <si>
@@ -47,392 +55,229 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>操作</t>
-    <rPh sb="0" eb="2">
-      <t>ソウサ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>アプリを起動</t>
-    <rPh sb="4" eb="6">
-      <t>キドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>登録ボタンを押下</t>
-    <rPh sb="0" eb="2">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>オウカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>状態</t>
-    <rPh sb="0" eb="2">
-      <t>ジョウタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・入力欄には何も表示されていないこと
-・テーブルは'支出'が選択されていること</t>
-    <rPh sb="1" eb="4">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>取消ボタンを押下</t>
-    <rPh sb="0" eb="2">
-      <t>トリケシ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>オウカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '100'
-ボタン: '収入'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
+    <t>InputChecker.checkEmrpty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InputChecker.checkDate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InputChecker.checkPrice</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date: '2015-01-01'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>price: 100</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.sendRequest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs:[
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="31" eb="32">
       <t>ヨウ</t>
     </rPh>
-    <rPh sb="43" eb="45">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-ボタン: '収入'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 201,
+  body: {
+    account_type: 'expense',
+    date: '2015-01-01',
+    content: 'テスト用データ',
+    category: 'テスト',
+    price: 100
+  }
+}</t>
+    <rPh sb="97" eb="98">
       <t>ヨウ</t>
     </rPh>
-    <rPh sb="37" eb="39">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・入力欄には何も表示されていないこと
-・テーブルは'収入'が選択されていること</t>
-    <rPh sb="1" eb="4">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'家計簿が登録されました'と表示されていること
-・テーブルは'収入'が選択されていること</t>
-    <rPh sb="2" eb="5">
-      <t>カケイボ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>シュウニュウ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs:[
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="31" eb="32">
       <t>ヨウ</t>
     </rPh>
-    <rPh sb="37" eb="39">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'カテゴリ, 金額を入力してください'と表示されていること
-・カテゴリの入力欄の横にマークが表示されていること
-・金額の入力欄の横にマークが表示されていること</t>
-    <rPh sb="8" eb="10">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="37" eb="40">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="61" eb="64">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'日付が不正です'と表示されていること
-・日付の入力欄の横にマークが表示されていること</t>
-    <rPh sb="2" eb="4">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="25" eb="28">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'金額が不正です'と表示されていること
-・金額の入力欄の横にマークが表示されていること</t>
-    <rPh sb="2" eb="4">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="25" eb="28">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '不正な日付'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '100'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InputChecker.checkEmpty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[3]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[0,1,2,3,4]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InputChecker.checkDate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Inputchecker.checkPrice</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date: 'invalid_date'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>price: 'invalid_price'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  'テスト用データ',
+  null,
+  '100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
       <t>ヨウ</t>
     </rPh>
-    <rPh sb="38" eb="40">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '2015-01-01'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '不正な金額'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.sendRequest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '01-01-2015',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
       <t>ヨウ</t>
     </rPh>
-    <rPh sb="43" eb="45">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日付: '01-01-2015'
-内容: 'テスト用データ'
-カテゴリ: 'テスト'
-金額: '-100'
-ボタン: '支出'を選択</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  null,
+  'テスト',
+  null,
+  'expense'
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [error_code: 'absent_param_category']
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [error_code: 'invalid_param_date']
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [
+      error_code: 'absent_param_content',
+      error_code: 'absent_param_price'
+    ]
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '01-01-2015',
+  'テスト用データ',
+  'テスト',
+  '-100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
       <t>ヨウ</t>
     </rPh>
-    <rPh sb="43" eb="45">
-      <t>キンガク</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [
+      error_code: 'invalid_param_date',
+      error_code: 'invalid_param_price'
+    ]
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  null,
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
     </rPh>
-    <rPh sb="60" eb="62">
-      <t>シシュツ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>センタク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・'日付, 金額が不正です'と表示されていること
-・日付の入力欄の横にマークが表示されていること
-・金額の入力欄の横にマークが表示されていること</t>
-    <rPh sb="2" eb="4">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>フセイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ヒヅケ</t>
-    </rPh>
-    <rPh sb="29" eb="32">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="53" eb="56">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>ヨコ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ヒョウジ</t>
-    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [null, null, null, null, null]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -735,7 +580,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -925,8 +770,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -954,14 +801,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -975,8 +825,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="191">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -1071,6 +924,7 @@
     <cellStyle name="ハイパーリンク" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1166,6 +1020,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="190" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1497,6 +1352,127 @@
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col min="6" max="7" width="47.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="19" thickBot="1"/>
+    <row r="2" spans="2:7" ht="19" thickBot="1">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="96">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="136" thickBot="1">
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1517,208 +1493,160 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="31">
-      <c r="B3" s="8">
+    <row r="3" spans="2:7" ht="96">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="15">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="96">
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="96">
+      <c r="B8" s="15">
         <v>6</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15" t="s">
-        <v>9</v>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="21" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="70">
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="10" t="s">
+    <row r="9" spans="2:7" ht="122">
+      <c r="B9" s="15">
         <v>7</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15" t="s">
-        <v>14</v>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="70">
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="45" thickBot="1">
-      <c r="B6" s="13">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="47.1640625" customWidth="1"/>
-    <col min="7" max="7" width="56.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="19" thickBot="1"/>
-    <row r="2" spans="2:7" ht="19" thickBot="1">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    <row r="10" spans="2:7" ht="123" thickBot="1">
+      <c r="B10" s="14">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="44">
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="70">
-      <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="70">
-      <c r="B5" s="14">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="71" thickBot="1">
-      <c r="B6" s="13">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19" t="s">
-        <v>22</v>
+      <c r="D10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>